<commit_message>
Tok også med midtdelere
</commit_message>
<xml_diff>
--- a/kostraleveranse2020/Kostra 20 - Midtrekkverk to og trefelts Fv.xlsx
+++ b/kostraleveranse2020/Kostra 20 - Midtrekkverk to og trefelts Fv.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,55 +452,71 @@
         <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>98</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>294</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>229</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B7" t="n">
-        <v>226</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>42</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>46</v>
+      </c>
+      <c r="B9" t="n">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>50</v>
       </c>
-      <c r="B8" t="n">
-        <v>70</v>
+      <c r="B10" t="n">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,55 +559,71 @@
         <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>930</v>
+        <v>6039</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>591</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>2793</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>744</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B7" t="n">
-        <v>520</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>42</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>46</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>50</v>
       </c>
-      <c r="B8" t="n">
-        <v>1598</v>
+      <c r="B10" t="n">
+        <v>2876</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -656,7 +688,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>66</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="3">
@@ -683,7 +715,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fv441</t>
+          <t>Fv47</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -692,7 +724,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>555</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5">
@@ -701,61 +733,61 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fv4852</t>
+          <t>Fv441</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2-3felt</t>
+          <t>mangefelt</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>32</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fv108</t>
+          <t>Fv507</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>mangefelt</t>
+          <t>2-3felt</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>296</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fv113</t>
+          <t>Fv554</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2-3felt</t>
+          <t>mangefelt</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fv156</t>
+          <t>Fv4848</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -764,34 +796,34 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>28</v>
+        <v>616</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fv282</t>
+          <t>Fv4848</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2-3felt</t>
+          <t>2-3felt,mangefelt</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>77</v>
+        <v>900</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fv283</t>
+          <t>Fv4852</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -800,16 +832,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>183</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fv33</t>
+          <t>Fv5928</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -818,16 +850,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>97</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fv51</t>
+          <t>Fv76</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -836,16 +868,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Fv300</t>
+          <t>Fv40</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -854,34 +886,34 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>97</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fv300</t>
+          <t>Fv108</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2-3felt,mangefelt</t>
+          <t>mangefelt</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1084</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fv300</t>
+          <t>Fv109</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -890,16 +922,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1479</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fv308</t>
+          <t>Fv113</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -908,16 +940,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Fv325</t>
+          <t>Fv120</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -926,16 +958,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Fv3106</t>
+          <t>Fv156</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -944,16 +976,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Fv3180</t>
+          <t>Fv164</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -962,34 +994,34 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Fv408</t>
+          <t>Fv164</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2-3felt</t>
+          <t>2-3felt,ukjent</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fv456</t>
+          <t>Fv166</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -998,52 +1030,52 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>636</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fv456</t>
+          <t>Fv178</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ukjent</t>
+          <t>2-3felt</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fv471</t>
+          <t>Fv180</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2-3felt</t>
+          <t>Ettfelt</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>104</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Fv552</t>
+          <t>Fv181</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1052,34 +1084,34 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>53</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fv557</t>
+          <t>Fv241</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ettfelt</t>
+          <t>2-3felt</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>293</v>
+        <v>480</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Fv5454</t>
+          <t>Fv282</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1088,52 +1120,52 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>173</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fv6658</t>
+          <t>Fv283</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>mangefelt</t>
+          <t>2-3felt</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>33</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Fv6664</t>
+          <t>Fv283</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2-3felt</t>
+          <t>2-3felt,mangefelt</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>17</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fv6668</t>
+          <t>Fv283</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1142,16 +1174,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fv6688</t>
+          <t>Fv286</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1160,60 +1192,726 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>40</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Fv6690</t>
+          <t>Fv2848</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>mangefelt</t>
+          <t>2-3felt</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1469</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Fv6690</t>
+          <t>Fv2874</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ukjent</t>
+          <t>2-3felt</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
+        <v>34</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Fv33</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Fv51</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>38</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Fv300</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>38</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Fv300</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2-3felt,mangefelt</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>38</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Fv300</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Fv305</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Fv308</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Fv313</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Ettfelt</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>38</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Fv325</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>38</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Fv360</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>38</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Fv364</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>38</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Fv3106</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>38</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Fv3180</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>42</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Fv408</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>42</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Fv421</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>42</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Fv456</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>42</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Fv456</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ukjent</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>42</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Fv471</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>42</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Fv4132</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>46</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Fv552</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>46</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Fv557</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Ettfelt</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>46</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Fv557</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ukjent</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>46</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Fv558</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2-3felt,mangefelt</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>46</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Fv558</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>46</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Fv562</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>46</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Fv585</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>46</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Fv5454</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
         <v>50</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Fv715</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>50</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Fv715</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2-3felt,ukjent</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>50</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Fv715</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ukjent</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>50</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Fv6658</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>50</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Fv6664</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>50</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Fv6668</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>50</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Fv6680</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>50</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Fv6688</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>50</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Fv6690</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>mangefelt</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>50</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Fv6690</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ukjent</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>50</v>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>Fv6802</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>2-3felt</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2-3felt</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1308,7 +2006,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>egenskap(1248)=11789</t>
+          <t>egenskap(1248)=11788 OR egenskap(1248)=11789</t>
         </is>
       </c>
     </row>

</xml_diff>